<commit_message>
Nightly build - rev.8
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -28,20 +28,20 @@
     <sheet state="visible" name="Credits" sheetId="23" r:id="rId25"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="1" name="Z_E862327B_85EF_4C3B_B3C4_5BE0490CA3B0_.wvu.FilterData">StoryText1!$B$1:$H$105</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_F35CD725_A175_42A1_8559_ACF7DFCE6881_.wvu.FilterData">StoryText1!$E$1:$E$105</definedName>
-    <definedName hidden="1" localSheetId="2" name="Z_205A6D3E_11A9_4340_983F_5BA7FED43E71_.wvu.FilterData">StoryText2!$B$1:$H$485</definedName>
-    <definedName hidden="1" localSheetId="3" name="Z_205A6D3E_11A9_4340_983F_5BA7FED43E71_.wvu.FilterData">StoryText3!$B$1:$H$532</definedName>
-    <definedName hidden="1" localSheetId="4" name="Z_205A6D3E_11A9_4340_983F_5BA7FED43E71_.wvu.FilterData">Snippet1!$B$1:$H$35</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_C46F569E_AF90_4926_819D_552287A45EEE_.wvu.FilterData">StoryText1!$E$1:$E$105</definedName>
-    <definedName hidden="1" localSheetId="2" name="Z_C46F569E_AF90_4926_819D_552287A45EEE_.wvu.FilterData">StoryText2!$B$1:$H$485</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_F809E1CB_56BE_4503_A575_DF9C7F7E01BA_.wvu.FilterData">StoryText1!$E$1:$E$105</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_F809E1CB_56BE_4503_A575_DF9C7F7E01BA_.wvu.FilterData">StoryText2!$B$1:$H$485</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_841ADE9F_C1A2_48DA_A5D8_B90BBF5ED91C_.wvu.FilterData">StoryText1!$B$1:$H$105</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_E3CAD23F_CF90_445C_89AC_3077DDE3EC91_.wvu.FilterData">StoryText1!$E$1:$E$105</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_CDE21143_29F8_4EAA_9BD8_57A9B40E72D2_.wvu.FilterData">StoryText2!$B$1:$H$485</definedName>
+    <definedName hidden="1" localSheetId="3" name="Z_CDE21143_29F8_4EAA_9BD8_57A9B40E72D2_.wvu.FilterData">StoryText3!$B$1:$H$532</definedName>
+    <definedName hidden="1" localSheetId="4" name="Z_CDE21143_29F8_4EAA_9BD8_57A9B40E72D2_.wvu.FilterData">Snippet1!$B$1:$H$35</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{C46F569E-AF90-4926-819D-552287A45EEE}" name="Chapter 0 (Prologue)"/>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{205A6D3E-11A9-4340-983F-5BA7FED43E71}" name="Sorted by location"/>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{F35CD725-A175-42A1-8559-ACF7DFCE6881}" name="Unidentified strings"/>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{E862327B-85EF-4C3B-B3C4-5BE0490CA3B0}" name="Chapter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{F809E1CB-56BE-4503-A575-DF9C7F7E01BA}" name="Chapter 0 (Prologue)"/>
+    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{CDE21143-29F8-4EAA-9BD8-57A9B40E72D2}" name="Sorted by location"/>
+    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{E3CAD23F-CF90-445C-89AC-3077DDE3EC91}" name="Unidentified strings"/>
+    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{841ADE9F-C1A2-48DA-A5D8-B90BBF5ED91C}" name="Chapter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -64,7 +64,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10437" uniqueCount="7715">
   <si>
-    <t>rev. 7</t>
+    <t>rev. 8</t>
   </si>
   <si>
     <t>Translation Status</t>
@@ -8303,10 +8303,10 @@
 おたがい ベストをつくしましょう</t>
   </si>
   <si>
-    <t>Huh? I feel like I've seen you before...who are you?
-Heh heh, what's wrong? You're staring pretty hard.
-No, it's not what you think...I was...
-In any case, let's both do our best!</t>
+    <t>&lt;@Hikaru&gt;Huh? I feel like I've seen you before...who are you?
+&lt;@Beauty&gt;Heh heh, what's wrong? You're staring pretty hard.
+&lt;@Hikaru&gt;No, it's not what you think...I was...
+&lt;@Beauty&gt;In any case, let's both do our best!</t>
   </si>
   <si>
     <t>6 - inside medarotsha - regional tourney beauty</t>
@@ -8322,7 +8322,7 @@
 また どこかで あいましょう♥</t>
   </si>
   <si>
-    <t>You've become very strong! 'Til we meet again!♥</t>
+    <t>&lt;@Beauty&gt;You've become very strong! 'Til we meet again!♥</t>
   </si>
   <si>
     <t>6 - inside medarotsha - regional tourney beauty -&gt; win</t>
@@ -8339,7 +8339,7 @@
 まちがっても きみには まけないよ</t>
   </si>
   <si>
-    <t>This place is like a garden to me..
+    <t>&lt;@Yuuki&gt;This place is like a garden to me..
 Which is why, I won't lose to you, no matter what!</t>
   </si>
   <si>
@@ -8356,7 +8356,7 @@
 まけるなんて・・・</t>
   </si>
   <si>
-    <t>I can't believe it... To lose now of all times...</t>
+    <t>&lt;@YuukiSad&gt;I can't believe it... To lose now of all times...</t>
   </si>
   <si>
     <t>6 - inside medarotsha - regional tourney yuuki -&gt; win</t>
@@ -8371,7 +8371,7 @@
     <t>さいこうの しあいだったよ</t>
   </si>
   <si>
-    <t>That was a great match.</t>
+    <t>&lt;@Yuuki&gt;That was a great match.</t>
   </si>
   <si>
     <t>6 - inside medarotsha - regional tourney yuuki -&gt; lose</t>
@@ -8679,7 +8679,7 @@
 あるのかい？</t>
   </si>
   <si>
-    <t>What is it? Is there something you want?</t>
+    <t>&lt;@Yuuki&gt;What is it? Is there something you want?</t>
   </si>
   <si>
     <t>3 - medarotsha area - yuuki's house yuuki</t>
@@ -8698,7 +8698,7 @@
 きみにも 1セット わけてあげよう</t>
   </si>
   <si>
-    <t>I'm gonna try out a new product in the next tournament.
+    <t>&lt;@Yuuki&gt;I'm gonna try out a new product in the next tournament.
 It's not good to blame your parts if you lose. Here, I'll give you a set too.</t>
   </si>
   <si>
@@ -8719,7 +8719,7 @@
 けっちゃくを つけよう</t>
   </si>
   <si>
-    <t>Listen, in the final tournament, you and I are gonna fight in the semifinals.
+    <t>&lt;@Yuuki&gt;Listen, in the final tournament, you and I are gonna fight in the semifinals.
 You better not lose 'til then.
 We'll finally settle it there.</t>
   </si>
@@ -8742,7 +8742,7 @@
 きょうは まんげつじゃないのか？</t>
   </si>
   <si>
-    <t>You want to fix a broken Medal?
+    <t>&lt;@Yuuki&gt;You want to fix a broken Medal?
 Well, a long time ago, my grandpa told me a story that if you place a Medal in the fountain at the Ruins on the night of a full moon, the Medal will be revived.
 Isn't tonight a full moon?</t>
   </si>
@@ -8758,7 +8758,8 @@
 みても うれしくないからな</t>
   </si>
   <si>
-    <t>You should hurry and fix your Medal. It bums me out when you're depressed.</t>
+    <t>&lt;@Yuuki&gt;You should hurry and fix your Medal.
+It bums me out when you're depressed.</t>
   </si>
   <si>
     <t>B-371</t>
@@ -8774,7 +8775,9 @@
 あいてをしてあげても いいよ</t>
   </si>
   <si>
-    <t>Your Medarot has grown. ...I guess it's expected.
+    <t>&lt;@Yuuki&gt;Your Medarot has grown.
+...
+I guess it's expected.
 Feel free to ask for a match anytime.</t>
   </si>
   <si>
@@ -8788,7 +8791,7 @@
 さあ うけとリたまえ</t>
   </si>
   <si>
-    <t>Hey, don't look so sad! Take it.</t>
+    <t>&lt;@Yuuki&gt;Hey, don't look so sad! Take it.</t>
   </si>
   <si>
     <t>B-373</t>
@@ -8800,7 +8803,7 @@
     <t>ボクは ライバルとして なさけないよ</t>
   </si>
   <si>
-    <t>Don't make me regret calling you my rival.</t>
+    <t>&lt;@Yuuki&gt;Don't make me regret calling you my rival.</t>
   </si>
   <si>
     <t>B-374</t>
@@ -49304,14 +49307,14 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F35CD725-A175-42A1-8559-ACF7DFCE6881}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{E3CAD23F-CF90-445C-89AC-3077DDE3EC91}" filter="1" showAutoFilter="1">
       <autoFilter ref="$E$1:$E$105">
         <filterColumn colId="0">
           <filters blank="1"/>
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{C46F569E-AF90-4926-819D-552287A45EEE}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{F809E1CB-56BE-4503-A575-DF9C7F7E01BA}" filter="1" showAutoFilter="1">
       <autoFilter ref="$E$1:$E$105">
         <filterColumn colId="0">
           <customFilters>
@@ -49320,7 +49323,7 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{E862327B-85EF-4C3B-B3C4-5BE0490CA3B0}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{841ADE9F-C1A2-48DA-A5D8-B90BBF5ED91C}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$105">
         <filterColumn colId="3">
           <customFilters>
@@ -62759,7 +62762,7 @@
       <c r="C377" s="17" t="s">
         <v>2143</v>
       </c>
-      <c r="D377" s="17" t="s">
+      <c r="D377" s="16" t="s">
         <v>2144</v>
       </c>
       <c r="E377" s="16" t="s">
@@ -62789,7 +62792,7 @@
       <c r="C378" s="17" t="s">
         <v>2148</v>
       </c>
-      <c r="D378" s="17" t="s">
+      <c r="D378" s="16" t="s">
         <v>2149</v>
       </c>
       <c r="E378" s="16" t="s">
@@ -62863,7 +62866,7 @@
       <c r="C381" s="17" t="s">
         <v>2163</v>
       </c>
-      <c r="D381" s="17" t="s">
+      <c r="D381" s="16" t="s">
         <v>2164</v>
       </c>
       <c r="E381" s="16" t="s">
@@ -63293,7 +63296,7 @@
       <c r="C398" s="17" t="s">
         <v>2246</v>
       </c>
-      <c r="D398" s="17" t="s">
+      <c r="D398" s="16" t="s">
         <v>2247</v>
       </c>
       <c r="E398" s="16" t="s">
@@ -63321,7 +63324,7 @@
       <c r="C399" s="17" t="s">
         <v>2251</v>
       </c>
-      <c r="D399" s="17" t="s">
+      <c r="D399" s="16" t="s">
         <v>2252</v>
       </c>
       <c r="E399" s="16" t="s">
@@ -63348,7 +63351,7 @@
       <c r="C400" s="17" t="s">
         <v>2256</v>
       </c>
-      <c r="D400" s="17" t="s">
+      <c r="D400" s="16" t="s">
         <v>2257</v>
       </c>
       <c r="E400" s="18"/>
@@ -63377,7 +63380,7 @@
       <c r="C401" s="17" t="s">
         <v>2260</v>
       </c>
-      <c r="D401" s="17" t="s">
+      <c r="D401" s="16" t="s">
         <v>2261</v>
       </c>
       <c r="E401" s="18"/>
@@ -63385,8 +63388,9 @@
       <c r="G401" s="18" t="str">
         <f t="shared" si="1"/>
         <v>You should hurry and fix your
-Medal. It bums me out when
-you're depressed. </v>
+Medal. 
+It bums me out when you're
+depressed. </v>
       </c>
       <c r="H401" s="18"/>
     </row>
@@ -63400,15 +63404,16 @@
       <c r="C402" s="17" t="s">
         <v>2264</v>
       </c>
-      <c r="D402" s="17" t="s">
+      <c r="D402" s="16" t="s">
         <v>2265</v>
       </c>
       <c r="E402" s="18"/>
       <c r="F402" s="18"/>
       <c r="G402" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>Your Medarot has grown. ...I
-guess it's expected. 
+        <v>Your Medarot has grown. 
+... 
+I guess it's expected. 
 Feel free to ask for a match
 anytime. </v>
       </c>
@@ -63424,7 +63429,7 @@
       <c r="C403" s="17" t="s">
         <v>2268</v>
       </c>
-      <c r="D403" s="17" t="s">
+      <c r="D403" s="16" t="s">
         <v>2269</v>
       </c>
       <c r="E403" s="18"/>
@@ -63445,7 +63450,7 @@
       <c r="C404" s="17" t="s">
         <v>2272</v>
       </c>
-      <c r="D404" s="17" t="s">
+      <c r="D404" s="16" t="s">
         <v>2273</v>
       </c>
       <c r="E404" s="18"/>
@@ -65460,7 +65465,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C46F569E-AF90-4926-819D-552287A45EEE}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{F809E1CB-56BE-4503-A575-DF9C7F7E01BA}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$485">
         <filterColumn colId="3">
           <customFilters>
@@ -65469,7 +65474,7 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{205A6D3E-11A9-4340-983F-5BA7FED43E71}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{CDE21143-29F8-4EAA-9BD8-57A9B40E72D2}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$485">
         <sortState ref="B1:H485">
           <sortCondition ref="E1:E485"/>
@@ -78368,7 +78373,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{205A6D3E-11A9-4340-983F-5BA7FED43E71}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{CDE21143-29F8-4EAA-9BD8-57A9B40E72D2}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$532">
         <sortState ref="B1:H532">
           <sortCondition ref="E1:E532"/>
@@ -79269,7 +79274,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{205A6D3E-11A9-4340-983F-5BA7FED43E71}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{CDE21143-29F8-4EAA-9BD8-57A9B40E72D2}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$35">
         <sortState ref="B1:H35">
           <sortCondition ref="E1:E35"/>

</xml_diff>

<commit_message>
Nightly build - rev. 9
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -28,20 +28,20 @@
     <sheet state="visible" name="Credits" sheetId="23" r:id="rId25"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="1" name="Z_42ACBEE9_9723_412C_AFD4_EEE36BB9DEB9_.wvu.FilterData">StoryText1!$E$1:$E$105</definedName>
-    <definedName hidden="1" localSheetId="2" name="Z_42ACBEE9_9723_412C_AFD4_EEE36BB9DEB9_.wvu.FilterData">StoryText2!$B$1:$H$485</definedName>
-    <definedName hidden="1" localSheetId="2" name="Z_82262917_3688_4057_ABEE_DC8AF9B7255A_.wvu.FilterData">StoryText2!$B$1:$H$485</definedName>
-    <definedName hidden="1" localSheetId="3" name="Z_82262917_3688_4057_ABEE_DC8AF9B7255A_.wvu.FilterData">StoryText3!$B$1:$H$532</definedName>
-    <definedName hidden="1" localSheetId="4" name="Z_82262917_3688_4057_ABEE_DC8AF9B7255A_.wvu.FilterData">Snippet1!$B$1:$H$35</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_4CDE152C_C3C5_472D_8122_8A8385BCBB65_.wvu.FilterData">StoryText1!$B$1:$H$105</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_E31B94E6_7CDA_4947_8BAD_A9195C7E9B8D_.wvu.FilterData">StoryText1!$E$1:$E$105</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_E3773B10_3D88_450E_B5D5_124693DBC50B_.wvu.FilterData">StoryText1!$B$1:$H$105</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_D5336419_E3CB_4F64_960A_EB6668FC55E7_.wvu.FilterData">StoryText2!$B$1:$H$485</definedName>
+    <definedName hidden="1" localSheetId="3" name="Z_D5336419_E3CB_4F64_960A_EB6668FC55E7_.wvu.FilterData">StoryText3!$B$1:$H$532</definedName>
+    <definedName hidden="1" localSheetId="4" name="Z_D5336419_E3CB_4F64_960A_EB6668FC55E7_.wvu.FilterData">Snippet1!$B$1:$H$35</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_31D3E495_9170_4B76_AF56_78EFA880F7C9_.wvu.FilterData">StoryText1!$E$1:$E$105</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_7B92790E_0727_4944_9A1B_CE3A277EC056_.wvu.FilterData">StoryText1!$E$1:$E$105</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_7B92790E_0727_4944_9A1B_CE3A277EC056_.wvu.FilterData">StoryText2!$B$1:$H$485</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{42ACBEE9-9723-412C-AFD4-EEE36BB9DEB9}" name="Chapter 0 (Prologue)"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{82262917-3688-4057-ABEE-DC8AF9B7255A}" name="Sorted by location"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E31B94E6-7CDA-4947-8BAD-A9195C7E9B8D}" name="Unidentified strings"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4CDE152C-C3C5-472D-8122-8A8385BCBB65}" name="Chapter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{7B92790E-0727-4944-9A1B-CE3A277EC056}" name="Chapter 0 (Prologue)"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D5336419-E3CB-4F64-960A-EB6668FC55E7}" name="Sorted by location"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{31D3E495-9170-4B76-AF56-78EFA880F7C9}" name="Unidentified strings"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E3773B10-3D88-450E-B5D5-124693DBC50B}" name="Chapter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -64,7 +64,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10554" uniqueCount="7795">
   <si>
-    <t>rev. 8</t>
+    <t>rev. 9</t>
   </si>
   <si>
     <t>Translation Status</t>
@@ -11650,7 +11650,7 @@
 あんまリ あぶないことしちゃ だめよ</t>
   </si>
   <si>
-    <t>Medarots can quickly repair themselves after a Robottle, but it won't be so easy if one of you children gets hurt.
+    <t>&lt;@Nurse&gt;Medarots can quickly repair themselves after a Robottle, but it won't be so easy if one of you children gets hurt.
 Be sure to stay safe, alright?</t>
   </si>
   <si>
@@ -11669,7 +11669,7 @@
 いつか おあいて してくれる？</t>
   </si>
   <si>
-    <t>You may not have guessed it, but even I have a Medarot of my own.
+    <t>&lt;@Nurse&gt;You may not have guessed it, but even I have a Medarot of my own.
 She's a real cutie! ♥
 My Medarot is a type that specializes in repairs.
 Perhaps I'll bring her in sometime?</t>
@@ -11691,7 +11691,7 @@
 してくれって たのまれてるの</t>
   </si>
   <si>
-    <t>Oh, &lt;&amp;NAME&gt;! Hello.
+    <t>&lt;@Nurse&gt;Oh, &lt;&amp;NAME&gt;! Hello.
 Congratulations on winning the tournament.
 Your teacher would like to do some special training with you and Yuuki.</t>
   </si>
@@ -11711,7 +11711,7 @@
 こころの じゅんびは いい？&lt;*4&gt;</t>
   </si>
   <si>
-    <t>I'm not sure if I'll be of any help but I'd be glad to.
+    <t>&lt;@Nurse&gt;I'm not sure if I'll be of any help but I'd be glad to.
 So, are you ready?&lt;*4&gt;</t>
   </si>
   <si>
@@ -11726,7 +11726,7 @@
 でも ムチャだけは しちゃだめよ</t>
   </si>
   <si>
-    <t>If you like, I could lend you my Medal.
+    <t>&lt;@Nurse&gt;If you like, I could lend you my Medal.
 But don't do anything reckless with it!</t>
   </si>
   <si>
@@ -28349,7 +28349,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="0" name="image3.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28377,7 +28377,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png"/>
+        <xdr:cNvPr id="0" name="image7.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28405,7 +28405,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png"/>
+        <xdr:cNvPr id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28433,7 +28433,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="0" name="image9.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28461,7 +28461,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png"/>
+        <xdr:cNvPr id="0" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28489,7 +28489,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png"/>
+        <xdr:cNvPr id="0" name="image5.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28545,7 +28545,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image15.png"/>
+        <xdr:cNvPr id="0" name="image14.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28573,7 +28573,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image13.png"/>
+        <xdr:cNvPr id="0" name="image18.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28601,7 +28601,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image16.png"/>
+        <xdr:cNvPr id="0" name="image8.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28629,7 +28629,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image21.png"/>
+        <xdr:cNvPr id="0" name="image15.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28657,7 +28657,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image19.png"/>
+        <xdr:cNvPr id="0" name="image22.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28685,7 +28685,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image18.png"/>
+        <xdr:cNvPr id="0" name="image19.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28713,7 +28713,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image23.png"/>
+        <xdr:cNvPr id="0" name="image24.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28741,7 +28741,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.png"/>
+        <xdr:cNvPr id="0" name="image13.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28769,7 +28769,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png"/>
+        <xdr:cNvPr id="0" name="image11.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28825,7 +28825,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image22.png"/>
+        <xdr:cNvPr id="0" name="image16.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28853,7 +28853,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png"/>
+        <xdr:cNvPr id="0" name="image10.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28881,7 +28881,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image20.png"/>
+        <xdr:cNvPr id="0" name="image23.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28909,7 +28909,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png"/>
+        <xdr:cNvPr id="0" name="image6.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28937,7 +28937,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png"/>
+        <xdr:cNvPr id="0" name="image12.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28965,7 +28965,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image24.png"/>
+        <xdr:cNvPr id="0" name="image21.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28993,7 +28993,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png"/>
+        <xdr:cNvPr id="0" name="image20.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -51030,14 +51030,14 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E31B94E6-7CDA-4947-8BAD-A9195C7E9B8D}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{31D3E495-9170-4B76-AF56-78EFA880F7C9}" filter="1" showAutoFilter="1">
       <autoFilter ref="$E$1:$E$105">
         <filterColumn colId="0">
           <filters blank="1"/>
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{42ACBEE9-9723-412C-AFD4-EEE36BB9DEB9}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{7B92790E-0727-4944-9A1B-CE3A277EC056}" filter="1" showAutoFilter="1">
       <autoFilter ref="$E$1:$E$105">
         <filterColumn colId="0">
           <customFilters>
@@ -51046,7 +51046,7 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{4CDE152C-C3C5-472D-8122-8A8385BCBB65}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{E3773B10-3D88-450E-B5D5-124693DBC50B}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$105">
         <filterColumn colId="3">
           <customFilters>
@@ -67188,7 +67188,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{42ACBEE9-9723-412C-AFD4-EEE36BB9DEB9}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{7B92790E-0727-4944-9A1B-CE3A277EC056}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$485">
         <filterColumn colId="3">
           <customFilters>
@@ -67197,7 +67197,7 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{82262917-3688-4057-ABEE-DC8AF9B7255A}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{D5336419-E3CB-4F64-960A-EB6668FC55E7}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$485">
         <sortState ref="B1:H485">
           <sortCondition ref="E1:E485"/>
@@ -69445,7 +69445,7 @@
       <c r="C89" s="19" t="s">
         <v>3038</v>
       </c>
-      <c r="D89" s="19" t="s">
+      <c r="D89" s="18" t="s">
         <v>3039</v>
       </c>
       <c r="E89" s="18" t="s">
@@ -69504,7 +69504,7 @@
       <c r="C91" s="19" t="s">
         <v>3047</v>
       </c>
-      <c r="D91" s="19" t="s">
+      <c r="D91" s="18" t="s">
         <v>3048</v>
       </c>
       <c r="E91" s="18" t="s">
@@ -69532,7 +69532,7 @@
       <c r="C92" s="19" t="s">
         <v>3052</v>
       </c>
-      <c r="D92" s="19" t="s">
+      <c r="D92" s="18" t="s">
         <v>3053</v>
       </c>
       <c r="E92" s="18" t="s">
@@ -69557,7 +69557,7 @@
       <c r="C93" s="19" t="s">
         <v>3056</v>
       </c>
-      <c r="D93" s="19" t="s">
+      <c r="D93" s="18" t="s">
         <v>3057</v>
       </c>
       <c r="E93" s="18" t="s">
@@ -80098,7 +80098,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{82262917-3688-4057-ABEE-DC8AF9B7255A}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{D5336419-E3CB-4F64-960A-EB6668FC55E7}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$532">
         <sortState ref="B1:H532">
           <sortCondition ref="E1:E532"/>
@@ -80995,7 +80995,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{82262917-3688-4057-ABEE-DC8AF9B7255A}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{D5336419-E3CB-4F64-960A-EB6668FC55E7}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$35">
         <sortState ref="B1:H35">
           <sortCondition ref="E1:E35"/>

</xml_diff>

<commit_message>
Nightly build - rev. 12
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -28,20 +28,20 @@
     <sheet state="visible" name="Credits" sheetId="23" r:id="rId25"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="1" name="Z_0E145B76_2136_4C14_995B_EA4F767742F8_.wvu.FilterData">StoryText1!$E$1:$E$105</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_E5F0296A_86A4_471D_8455_1294AE72CAB4_.wvu.FilterData">StoryText1!$B$1:$H$105</definedName>
-    <definedName hidden="1" localSheetId="2" name="Z_DFF92B95_7C86_4DC7_A56A_2FBF6472CDEE_.wvu.FilterData">StoryText2!$B$1:$H$485</definedName>
-    <definedName hidden="1" localSheetId="3" name="Z_DFF92B95_7C86_4DC7_A56A_2FBF6472CDEE_.wvu.FilterData">StoryText3!$B$1:$H$532</definedName>
-    <definedName hidden="1" localSheetId="4" name="Z_DFF92B95_7C86_4DC7_A56A_2FBF6472CDEE_.wvu.FilterData">Snippet1!$B$1:$H$35</definedName>
-    <definedName hidden="1" localSheetId="1" name="Z_3FA84059_40DC_436B_9978_74DA36EFD166_.wvu.FilterData">StoryText1!$E$1:$E$105</definedName>
-    <definedName hidden="1" localSheetId="2" name="Z_3FA84059_40DC_436B_9978_74DA36EFD166_.wvu.FilterData">StoryText2!$B$1:$H$485</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_099C57BE_893F_4950_B0B5_993A63932B30_.wvu.FilterData">StoryText1!$E$1:$E$105</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_099C57BE_893F_4950_B0B5_993A63932B30_.wvu.FilterData">StoryText2!$B$1:$H$485</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_585373CF_EA9A_467E_8C7B_FB81F14BC17D_.wvu.FilterData">StoryText1!$E$1:$E$105</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_28273F8B_3E17_4AC2_8273_8CD6B409C35F_.wvu.FilterData">StoryText2!$B$1:$H$485</definedName>
+    <definedName hidden="1" localSheetId="3" name="Z_28273F8B_3E17_4AC2_8273_8CD6B409C35F_.wvu.FilterData">StoryText3!$B$1:$H$532</definedName>
+    <definedName hidden="1" localSheetId="4" name="Z_28273F8B_3E17_4AC2_8273_8CD6B409C35F_.wvu.FilterData">Snippet1!$B$1:$H$35</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_1540C16D_1267_4B2C_8430_31D16AC78496_.wvu.FilterData">StoryText1!$B$1:$H$105</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{3FA84059-40DC-436B-9978-74DA36EFD166}" name="Chapter 0 (Prologue)"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DFF92B95-7C86-4DC7-A56A-2FBF6472CDEE}" name="Sorted by location"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0E145B76-2136-4C14-995B-EA4F767742F8}" name="Unidentified strings"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E5F0296A-86A4-471D-8455-1294AE72CAB4}" name="Chapter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{099C57BE-893F-4950-B0B5-993A63932B30}" name="Chapter 0 (Prologue)"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{28273F8B-3E17-4AC2-8273-8CD6B409C35F}" name="Sorted by location"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{585373CF-EA9A-467E-8C7B-FB81F14BC17D}" name="Unidentified strings"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{1540C16D-1267-4B2C-8430-31D16AC78496}" name="Chapter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -64,7 +64,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10555" uniqueCount="7797">
   <si>
-    <t>rev. 11</t>
+    <t>rev. 12</t>
   </si>
   <si>
     <t>Translation Status</t>
@@ -20188,7 +20188,7 @@
 よろしいですか？&lt;*4&gt;</t>
   </si>
   <si>
-    <t>Are you sure you want to throw it away?</t>
+    <t>Are you sure you want to throw it away? &lt;*4&gt;</t>
   </si>
   <si>
     <t>Tossing items confirmation</t>
@@ -28366,7 +28366,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="0" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28394,7 +28394,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png"/>
+        <xdr:cNvPr id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28422,7 +28422,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="0" name="image4.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28450,7 +28450,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image16.png"/>
+        <xdr:cNvPr id="0" name="image22.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28478,7 +28478,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png"/>
+        <xdr:cNvPr id="0" name="image5.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28506,7 +28506,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png"/>
+        <xdr:cNvPr id="0" name="image19.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28534,7 +28534,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image29.png"/>
+        <xdr:cNvPr id="0" name="image20.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28562,7 +28562,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png"/>
+        <xdr:cNvPr id="0" name="image9.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28590,7 +28590,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image20.png"/>
+        <xdr:cNvPr id="0" name="image13.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28618,7 +28618,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image22.png"/>
+        <xdr:cNvPr id="0" name="image3.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28646,7 +28646,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image17.png"/>
+        <xdr:cNvPr id="0" name="image23.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28674,7 +28674,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image21.png"/>
+        <xdr:cNvPr id="0" name="image17.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28730,7 +28730,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image15.png"/>
+        <xdr:cNvPr id="0" name="image12.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28758,7 +28758,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png"/>
+        <xdr:cNvPr id="0" name="image24.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28786,7 +28786,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png"/>
+        <xdr:cNvPr id="0" name="image14.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28814,7 +28814,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image23.png"/>
+        <xdr:cNvPr id="0" name="image21.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28842,7 +28842,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image27.png"/>
+        <xdr:cNvPr id="0" name="image25.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28870,7 +28870,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image26.png"/>
+        <xdr:cNvPr id="0" name="image11.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28898,7 +28898,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png"/>
+        <xdr:cNvPr id="0" name="image10.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28926,7 +28926,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png"/>
+        <xdr:cNvPr id="0" name="image7.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28954,7 +28954,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png"/>
+        <xdr:cNvPr id="0" name="image8.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -28982,7 +28982,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image13.png"/>
+        <xdr:cNvPr id="0" name="image6.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29010,7 +29010,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.png"/>
+        <xdr:cNvPr id="0" name="image16.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29038,7 +29038,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image24.png"/>
+        <xdr:cNvPr id="0" name="image15.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29066,7 +29066,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png"/>
+        <xdr:cNvPr id="0" name="image26.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29094,7 +29094,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image25.png"/>
+        <xdr:cNvPr id="0" name="image31.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29122,7 +29122,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image19.png"/>
+        <xdr:cNvPr id="0" name="image29.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29150,7 +29150,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image28.png"/>
+        <xdr:cNvPr id="0" name="image33.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29178,7 +29178,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image30.png"/>
+        <xdr:cNvPr id="0" name="image28.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29206,7 +29206,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image49.png"/>
+        <xdr:cNvPr id="0" name="image38.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29234,7 +29234,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image40.png"/>
+        <xdr:cNvPr id="0" name="image30.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29262,7 +29262,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image37.png"/>
+        <xdr:cNvPr id="0" name="image45.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29290,7 +29290,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image34.png"/>
+        <xdr:cNvPr id="0" name="image35.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29318,7 +29318,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image32.png"/>
+        <xdr:cNvPr id="0" name="image36.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29346,7 +29346,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image31.png"/>
+        <xdr:cNvPr id="0" name="image32.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29374,7 +29374,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image42.png"/>
+        <xdr:cNvPr id="0" name="image27.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29402,7 +29402,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image33.png"/>
+        <xdr:cNvPr id="0" name="image51.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29430,7 +29430,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image53.png"/>
+        <xdr:cNvPr id="0" name="image41.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29486,7 +29486,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image38.png"/>
+        <xdr:cNvPr id="0" name="image46.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29514,7 +29514,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image35.png"/>
+        <xdr:cNvPr id="0" name="image39.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29542,7 +29542,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image41.png"/>
+        <xdr:cNvPr id="0" name="image48.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29570,7 +29570,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image45.png"/>
+        <xdr:cNvPr id="0" name="image40.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29598,7 +29598,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image36.png"/>
+        <xdr:cNvPr id="0" name="image37.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29626,7 +29626,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image46.png"/>
+        <xdr:cNvPr id="0" name="image34.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29654,7 +29654,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image52.png"/>
+        <xdr:cNvPr id="0" name="image49.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29682,7 +29682,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image48.png"/>
+        <xdr:cNvPr id="0" name="image47.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29710,7 +29710,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image39.png"/>
+        <xdr:cNvPr id="0" name="image42.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29738,7 +29738,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image47.png"/>
+        <xdr:cNvPr id="0" name="image43.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29766,7 +29766,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image43.png"/>
+        <xdr:cNvPr id="0" name="image50.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29794,7 +29794,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image51.png"/>
+        <xdr:cNvPr id="0" name="image94.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29822,7 +29822,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image50.png"/>
+        <xdr:cNvPr id="0" name="image53.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29850,7 +29850,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image56.png"/>
+        <xdr:cNvPr id="0" name="image55.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29878,7 +29878,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image54.png"/>
+        <xdr:cNvPr id="0" name="image58.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29906,7 +29906,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image60.png"/>
+        <xdr:cNvPr id="0" name="image63.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29934,7 +29934,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image55.png"/>
+        <xdr:cNvPr id="0" name="image65.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -29962,7 +29962,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image65.png"/>
+        <xdr:cNvPr id="0" name="image57.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30018,7 +30018,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image63.png"/>
+        <xdr:cNvPr id="0" name="image69.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30046,7 +30046,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image70.png"/>
+        <xdr:cNvPr id="0" name="image52.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30074,7 +30074,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image68.png"/>
+        <xdr:cNvPr id="0" name="image56.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30102,7 +30102,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image72.png"/>
+        <xdr:cNvPr id="0" name="image71.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30130,7 +30130,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image62.png"/>
+        <xdr:cNvPr id="0" name="image68.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30158,7 +30158,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image67.png"/>
+        <xdr:cNvPr id="0" name="image54.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30186,7 +30186,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image57.png"/>
+        <xdr:cNvPr id="0" name="image66.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30214,7 +30214,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image58.png"/>
+        <xdr:cNvPr id="0" name="image79.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30242,7 +30242,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image61.png"/>
+        <xdr:cNvPr id="0" name="image64.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30270,7 +30270,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image64.png"/>
+        <xdr:cNvPr id="0" name="image61.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30298,7 +30298,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image69.png"/>
+        <xdr:cNvPr id="0" name="image62.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30326,7 +30326,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image71.png"/>
+        <xdr:cNvPr id="0" name="image60.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30354,7 +30354,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image76.png"/>
+        <xdr:cNvPr id="0" name="image70.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30410,7 +30410,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image66.png"/>
+        <xdr:cNvPr id="0" name="image72.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30438,7 +30438,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image74.png"/>
+        <xdr:cNvPr id="0" name="image67.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30466,7 +30466,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image81.png"/>
+        <xdr:cNvPr id="0" name="image75.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30494,7 +30494,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image78.png"/>
+        <xdr:cNvPr id="0" name="image80.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30522,7 +30522,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image79.png"/>
+        <xdr:cNvPr id="0" name="image74.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30550,7 +30550,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image75.png"/>
+        <xdr:cNvPr id="0" name="image77.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30578,7 +30578,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image77.png"/>
+        <xdr:cNvPr id="0" name="image92.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30606,7 +30606,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image82.png"/>
+        <xdr:cNvPr id="0" name="image76.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30634,7 +30634,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image96.png"/>
+        <xdr:cNvPr id="0" name="image85.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30662,7 +30662,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image80.png"/>
+        <xdr:cNvPr id="0" name="image89.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30690,7 +30690,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image88.png"/>
+        <xdr:cNvPr id="0" name="image81.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30718,7 +30718,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image83.png"/>
+        <xdr:cNvPr id="0" name="image84.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30746,7 +30746,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image90.png"/>
+        <xdr:cNvPr id="0" name="image83.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30774,7 +30774,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image92.png"/>
+        <xdr:cNvPr id="0" name="image86.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30802,7 +30802,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image87.png"/>
+        <xdr:cNvPr id="0" name="image78.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30830,7 +30830,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image91.png"/>
+        <xdr:cNvPr id="0" name="image88.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30858,7 +30858,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image94.png"/>
+        <xdr:cNvPr id="0" name="image82.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30886,7 +30886,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image93.png"/>
+        <xdr:cNvPr id="0" name="image98.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30914,7 +30914,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image89.png"/>
+        <xdr:cNvPr id="0" name="image93.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30942,7 +30942,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image84.png"/>
+        <xdr:cNvPr id="0" name="image87.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30970,7 +30970,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image95.png"/>
+        <xdr:cNvPr id="0" name="image91.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -30998,7 +30998,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image86.png"/>
+        <xdr:cNvPr id="0" name="image96.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31026,7 +31026,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image85.png"/>
+        <xdr:cNvPr id="0" name="image103.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31054,7 +31054,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image98.png"/>
+        <xdr:cNvPr id="0" name="image107.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31082,7 +31082,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image99.png"/>
+        <xdr:cNvPr id="0" name="image97.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31110,7 +31110,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image108.png"/>
+        <xdr:cNvPr id="0" name="image100.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31138,7 +31138,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image104.png"/>
+        <xdr:cNvPr id="0" name="image90.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31166,7 +31166,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image100.png"/>
+        <xdr:cNvPr id="0" name="image105.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31194,7 +31194,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image97.png"/>
+        <xdr:cNvPr id="0" name="image95.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31222,7 +31222,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image101.png"/>
+        <xdr:cNvPr id="0" name="image110.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31250,7 +31250,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image102.png"/>
+        <xdr:cNvPr id="0" name="image104.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31278,7 +31278,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image114.png"/>
+        <xdr:cNvPr id="0" name="image108.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31306,7 +31306,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image107.png"/>
+        <xdr:cNvPr id="0" name="image101.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31334,7 +31334,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image103.png"/>
+        <xdr:cNvPr id="0" name="image99.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31390,7 +31390,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image109.png"/>
+        <xdr:cNvPr id="0" name="image111.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31418,7 +31418,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image110.png"/>
+        <xdr:cNvPr id="0" name="image112.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31446,7 +31446,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image112.png"/>
+        <xdr:cNvPr id="0" name="image109.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31474,7 +31474,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image111.png"/>
+        <xdr:cNvPr id="0" name="image102.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -31502,7 +31502,7 @@
     <xdr:ext cx="200025" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image105.png"/>
+        <xdr:cNvPr id="0" name="image114.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -36112,7 +36112,7 @@
       <c r="B131" s="22" t="s">
         <v>5377</v>
       </c>
-      <c r="C131" s="22" t="s">
+      <c r="C131" s="21" t="s">
         <v>5378</v>
       </c>
       <c r="D131" s="21" t="s">
@@ -36122,7 +36122,7 @@
       <c r="F131" s="21" t="str">
         <f t="shared" si="4"/>
         <v>Are you sure you want to
-throw it away? </v>
+throw it away?  </v>
       </c>
       <c r="G131" s="23"/>
     </row>
@@ -53939,14 +53939,14 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{0E145B76-2136-4C14-995B-EA4F767742F8}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{585373CF-EA9A-467E-8C7B-FB81F14BC17D}" filter="1" showAutoFilter="1">
       <autoFilter ref="$E$1:$E$105">
         <filterColumn colId="0">
           <filters blank="1"/>
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{3FA84059-40DC-436B-9978-74DA36EFD166}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{099C57BE-893F-4950-B0B5-993A63932B30}" filter="1" showAutoFilter="1">
       <autoFilter ref="$E$1:$E$105">
         <filterColumn colId="0">
           <customFilters>
@@ -53955,7 +53955,7 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{E5F0296A-86A4-471D-8455-1294AE72CAB4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{1540C16D-1267-4B2C-8430-31D16AC78496}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$105">
         <filterColumn colId="3">
           <customFilters>
@@ -70097,7 +70097,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3FA84059-40DC-436B-9978-74DA36EFD166}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{099C57BE-893F-4950-B0B5-993A63932B30}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$485">
         <filterColumn colId="3">
           <customFilters>
@@ -70106,7 +70106,7 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{DFF92B95-7C86-4DC7-A56A-2FBF6472CDEE}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{28273F8B-3E17-4AC2-8273-8CD6B409C35F}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$485">
         <sortState ref="B1:H485">
           <sortCondition ref="E1:E485"/>
@@ -83007,7 +83007,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DFF92B95-7C86-4DC7-A56A-2FBF6472CDEE}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{28273F8B-3E17-4AC2-8273-8CD6B409C35F}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$532">
         <sortState ref="B1:H532">
           <sortCondition ref="E1:E532"/>
@@ -83904,7 +83904,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DFF92B95-7C86-4DC7-A56A-2FBF6472CDEE}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{28273F8B-3E17-4AC2-8273-8CD6B409C35F}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$H$35">
         <sortState ref="B1:H35">
           <sortCondition ref="E1:E35"/>

</xml_diff>